<commit_message>
Moved figures to manuscript. Create statistics of papers
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/Round 2/RQ1_Round2_0.0.1.xlsx
+++ b/DataExtraction/Extracted Data/Round 2/RQ1_Round2_0.0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/Projects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/Extracted Data/Round 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113CA335-407C-C94A-9375-1BA5EB36EF2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752273D8-668F-5A46-A31A-8C5F7A425E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="33600" windowHeight="21000" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -18,11 +18,11 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RQ1'!$F$1:$I$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RQ1'!$F$1:$I$121</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="62" r:id="rId3"/>
+    <pivotCache cacheId="10" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3279,7 +3279,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7D70EF13-A283-3A48-9359-ECE0C9FA1031}" name="PivotTable1" cacheId="62" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7D70EF13-A283-3A48-9359-ECE0C9FA1031}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A133" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -4163,11 +4163,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F108" sqref="F108"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2:G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4239,7 +4240,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -4355,7 +4356,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -4413,7 +4414,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -4442,7 +4443,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -4471,7 +4472,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
@@ -4500,7 +4501,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
@@ -4529,7 +4530,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>44</v>
       </c>
@@ -4616,7 +4617,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>53</v>
       </c>
@@ -4645,7 +4646,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
@@ -4674,7 +4675,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>60</v>
       </c>
@@ -4703,7 +4704,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>63</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>66</v>
       </c>
@@ -4790,7 +4791,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>74</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>78</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>85</v>
       </c>
@@ -4906,7 +4907,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>89</v>
       </c>
@@ -4935,7 +4936,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>92</v>
       </c>
@@ -4964,7 +4965,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>95</v>
       </c>
@@ -4993,7 +4994,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>97</v>
       </c>
@@ -5022,7 +5023,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="160" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>101</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>104</v>
       </c>
@@ -5080,7 +5081,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>107</v>
       </c>
@@ -5196,7 +5197,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>119</v>
       </c>
@@ -5312,7 +5313,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>131</v>
       </c>
@@ -5370,7 +5371,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>136</v>
       </c>
@@ -5399,7 +5400,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>139</v>
       </c>
@@ -5428,7 +5429,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>142</v>
       </c>
@@ -5457,7 +5458,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>145</v>
       </c>
@@ -5515,7 +5516,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>152</v>
       </c>
@@ -5544,7 +5545,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>156</v>
       </c>
@@ -5573,7 +5574,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>159</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>163</v>
       </c>
@@ -5631,7 +5632,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>165</v>
       </c>
@@ -5660,7 +5661,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>167</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>181</v>
       </c>
@@ -5834,7 +5835,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>183</v>
       </c>
@@ -5863,7 +5864,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>185</v>
       </c>
@@ -5892,7 +5893,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>189</v>
       </c>
@@ -6008,7 +6009,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>200</v>
       </c>
@@ -6066,7 +6067,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>207</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>210</v>
       </c>
@@ -6124,7 +6125,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>213</v>
       </c>
@@ -6153,7 +6154,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>216</v>
       </c>
@@ -6182,7 +6183,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>219</v>
       </c>
@@ -6211,7 +6212,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>221</v>
       </c>
@@ -6240,7 +6241,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>224</v>
       </c>
@@ -6298,7 +6299,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>228</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
         <v>231</v>
       </c>
@@ -6385,7 +6386,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>239</v>
       </c>
@@ -6414,7 +6415,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>242</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>244</v>
       </c>
@@ -6501,7 +6502,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>250</v>
       </c>
@@ -6559,7 +6560,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
         <v>254</v>
       </c>
@@ -6588,7 +6589,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="81" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12" t="s">
         <v>266</v>
       </c>
@@ -6646,7 +6647,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>272</v>
       </c>
@@ -6675,7 +6676,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>275</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>278</v>
       </c>
@@ -6733,7 +6734,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>281</v>
       </c>
@@ -6791,7 +6792,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>287</v>
       </c>
@@ -6849,7 +6850,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>293</v>
       </c>
@@ -6878,7 +6879,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>296</v>
       </c>
@@ -6936,7 +6937,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>302</v>
       </c>
@@ -6994,7 +6995,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>308</v>
       </c>
@@ -7023,7 +7024,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>311</v>
       </c>
@@ -7052,7 +7053,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>314</v>
       </c>
@@ -7081,7 +7082,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>317</v>
       </c>
@@ -7110,7 +7111,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>320</v>
       </c>
@@ -7197,7 +7198,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>299</v>
       </c>
@@ -7284,7 +7285,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>338</v>
       </c>
@@ -7313,7 +7314,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>341</v>
       </c>
@@ -7342,7 +7343,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>344</v>
       </c>
@@ -7400,7 +7401,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
         <v>350</v>
       </c>
@@ -7429,7 +7430,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>353</v>
       </c>
@@ -7661,7 +7662,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>376</v>
       </c>
@@ -7691,7 +7692,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I83" xr:uid="{5DB9841F-836E-494C-BC18-0828E2E8D89A}"/>
+  <autoFilter ref="F1:I121" xr:uid="{5DB9841F-836E-494C-BC18-0828E2E8D89A}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Improve Quality; New Functionality"/>
+        <filter val="New Functionality"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>